<commit_message>
added images to the popups
</commit_message>
<xml_diff>
--- a/places.xlsx
+++ b/places.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1B4977-D210-48BE-B7F1-D7F7050C08D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C729BE-226E-44D6-8BBC-C22336862B89}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
   <si>
     <t>LAT</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Jan 30 2015</t>
   </si>
   <si>
-    <t>Ravens Game</t>
-  </si>
-  <si>
     <t>Visiting Jessica+Eric</t>
   </si>
   <si>
@@ -313,7 +310,130 @@
     <t>Mar 2 2014</t>
   </si>
   <si>
-    <t>C:\Users\Andrew\Desktop\github\foliumproj\12123.JPG</t>
+    <t>Andrew Met Bay's Dad</t>
+  </si>
+  <si>
+    <t>Fashion Island</t>
+  </si>
+  <si>
+    <t>Jan 18 2015</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/16728_10155171767845472_1736650083411801148_n.jpg?_nc_cat=107&amp;oh=edf479e4053b597573fcf1765180020d&amp;oe=5C189341" style="width:50%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10920900_10155126879570472_506276529898579401_n.jpg?_nc_cat=103&amp;oh=325bff7775418f093e37cd022126c77d&amp;oe=5C555DA0" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10881686_10155030956530472_4441633013622423410_n.jpg?_nc_cat=103&amp;oh=e58f2683328f99eb78da483e50a1f4ea&amp;oe=5C161DA9" style="width:auto;height:50%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10885494_10155029400610472_1878221333012357816_n.jpg?_nc_cat=102&amp;oh=85a5fa79dfce191fc20bdf623941de1b&amp;oe=5C51D77A" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>Bay First Day of Work</t>
+  </si>
+  <si>
+    <t>Gaysorn</t>
+  </si>
+  <si>
+    <t>Mar 24 2012</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/561353_192107217571601_153601725_n.jpg?_nc_cat=100&amp;oh=3b4512804ead9977b733f6fa11ef3b93&amp;oe=5C6082E1" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/417358_171325126316477_1304069161_n.jpg?_nc_cat=109&amp;oh=58e997770183716233a0ec215176cfef&amp;oe=5C43AAA2" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/428226_10151383224825472_531323711_n.jpg?_nc_cat=101&amp;oh=a7e47353b102b2243959b844b08cfba4&amp;oe=5C180695" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>First USA Halloween Together</t>
+  </si>
+  <si>
+    <t>Millersville, MD</t>
+  </si>
+  <si>
+    <t>Oct 31 2016</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/14900384_10157672410480472_3353697473017192986_n.jpg?_nc_cat=107&amp;oh=c08e298bcf3088af7364d936af9b0703&amp;oe=5C5452F6" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/14729164_10157628070480472_2549399823511176984_n.jpg?_nc_cat=100&amp;oh=79324822dc2394d1094dae018064a42c&amp;oe=5C5F0172" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/42723614_10161027530845472_2577854609603166208_o.jpg?_nc_cat=101&amp;oh=a472bcf0eeae2686bfddcb43936b6b57&amp;oe=5C51E650" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>First Ravens Game</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/42432207_10161011613560472_2542234869564440576_o.jpg?_nc_cat=103&amp;oh=6f1251f27b323f710f2e3de7e74c3a39&amp;oe=5C62BE92" style="width:auto;height:60%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10805803_10154901235105472_7608660262787893426_n.jpg?_nc_cat=104&amp;oh=78c247d666763496b1b9f18c3fcedd91&amp;oe=5C60A1AF" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10685582_10154732241745472_6024607142167467387_n.jpg?_nc_cat=102&amp;oh=1494f94ecde57f9a7f6be35ae035d80e&amp;oe=5C546BD2" style="width:75%;height:AUTO;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/19797_10155405886360472_1632482625524258935_n.jpg?_nc_cat=101&amp;oh=75f0df8f337a9b1a048ef1678054ad8f&amp;oe=5C16F224" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/535323_10156391993930472_1393915873010677955_n.jpg?_nc_cat=108&amp;oh=b0a1847e9b80f847e9a2f22960a389af&amp;oe=5C42B4E1" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/17799376_10158486995710472_1570977125754334957_n.jpg?_nc_cat=103&amp;oh=3054d3dd9fe0be69ebc6a09cec5401eb&amp;oe=5C484F56" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t31.0-8/12496376_10156554717550472_3394337341673659606_o.jpg?_nc_cat=106&amp;oh=38f0da4f5a7127e4401480bad1f9d49f&amp;oe=5C5D9CA8" style="width:auto;height:60%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/17884023_10158492207155472_1286082213450447941_n.jpg?_nc_cat=105&amp;oh=92ced4d4c9a36a466cf97e484202c356&amp;oe=5C54F831" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/528965_218234728292183_2005747330_n.jpg?_nc_cat=107&amp;oh=1cd5a80551172cb30ae422bbe734a4f7&amp;oe=5C5DDDE4" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/385763_231669023615420_1121748693_n.jpg?_nc_cat=103&amp;oh=e1cb77eb8620f763ed3fc89f424a797d&amp;oe=5C527BA1" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/1480765_10153573612775472_1070556733_n.jpg?_nc_cat=102&amp;oh=cadc3be04d7742460a7dc484a890f883&amp;oe=5C50E54E" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t31.0-8/1074534_423811754401145_1162936417_o.jpg?_nc_cat=104&amp;oh=5b56687fd9ca2cc6ec0aa47bf5ae7617&amp;oe=5C4E08B0" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/1150418_10153118999170472_1431542147_n.jpg?_nc_cat=109&amp;oh=d2b541447213917a362b8eb66a1d4aac&amp;oe=5C458CEF" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/62619_10152767099955472_1988822311_n.jpg?_nc_cat=101&amp;oh=ae74fa09b643a3852b35813df1e394a9&amp;oe=5C5F6944" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/574472_10152576450870472_454279356_n.jpg?_nc_cat=107&amp;oh=e726de4458c62b90213d36c0ccfa0e1e&amp;oe=5C62DAED" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t31.0-8/477295_385610101554644_562621180_o.jpg?_nc_cat=100&amp;oh=e49fcf645102e9c6cca7c0550580db7d&amp;oe=5C54B4B2" style="width:auto;height:70%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/602766_339962592786062_1066806054_n.jpg?_nc_cat=103&amp;oh=0e3c29c01785438bd16eff873ef152de&amp;oe=5C5DA752" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t31.0-8/1979285_10153886727100472_1085309532_o.jpg?_nc_cat=107&amp;oh=31e9fc95096a387c4b2d907136826ba2&amp;oe=5C52D13D" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/18101_10152289472765472_1687701262_n.jpg?_nc_cat=101&amp;oh=1bbd103f56c93587b117a0305416acab&amp;oe=5C145450" style="width:75%;height:auto;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10409453_10154891079400472_5213033156147697270_n.jpg?_nc_cat=110&amp;oh=cff33a22a879e4fcb2dc070e1158cfc4&amp;oe=5C4C8B49" style="width:auto;height:75%;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/1376413_10154800938795472_2721843062770153549_n.jpg?_nc_cat=107&amp;oh=6e4362e57bd46e9ce514be8b345159fb&amp;oe=5C5D351D" style="width:auto;height:75%"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="https://scontent-iad3-1.xx.fbcdn.net/v/t1.0-9/10614194_10154544650605472_4099051271521523930_n.jpg?_nc_cat=110&amp;oh=54995187b4c15656b162edffed059dbb&amp;oe=5C19A26C" style="width:75%;height:auto;"&gt;</t>
   </si>
 </sst>
 </file>
@@ -641,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -706,7 +826,7 @@
         <v>100.52347899999999</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -714,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -730,6 +850,9 @@
       </c>
       <c r="G3">
         <v>100.564849</v>
+      </c>
+      <c r="H3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,6 +877,9 @@
       <c r="G4">
         <v>100.504053</v>
       </c>
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -777,6 +903,9 @@
       <c r="G5">
         <v>100.605475</v>
       </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -786,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -799,6 +928,9 @@
       </c>
       <c r="G6">
         <v>-73.987368000000004</v>
+      </c>
+      <c r="H6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -822,6 +954,9 @@
       </c>
       <c r="G7">
         <v>-76.623553999999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,6 +981,9 @@
       <c r="G8">
         <v>101.56521499999999</v>
       </c>
+      <c r="H8" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -855,7 +993,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -868,6 +1006,9 @@
       </c>
       <c r="G9">
         <v>104.758782</v>
+      </c>
+      <c r="H9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -878,19 +1019,22 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>17.965122999999998</v>
       </c>
       <c r="G10">
         <v>102.624769</v>
+      </c>
+      <c r="H10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -901,7 +1045,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -914,6 +1058,9 @@
       </c>
       <c r="G11">
         <v>-76.848493000000005</v>
+      </c>
+      <c r="H11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -938,28 +1085,34 @@
       <c r="G12">
         <v>98.916342999999998</v>
       </c>
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13">
         <v>30.323791</v>
       </c>
       <c r="G13">
         <v>-81.637743999999998</v>
+      </c>
+      <c r="H13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,22 +1120,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14">
         <v>38.900188</v>
       </c>
       <c r="G14">
         <v>-77.036743999999999</v>
+      </c>
+      <c r="H14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,22 +1146,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <v>32.081389999999999</v>
       </c>
       <c r="G15">
         <v>-81.089958999999993</v>
+      </c>
+      <c r="H15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1013,10 +1172,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
@@ -1030,22 +1189,25 @@
       <c r="G16">
         <v>-90.184984999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>13.724538000000001</v>
@@ -1053,22 +1215,25 @@
       <c r="G17" s="3">
         <v>100.581985</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
         <v>57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18">
         <v>13.754352000000001</v>
@@ -1076,22 +1241,25 @@
       <c r="G18">
         <v>100.54038</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>13.693174000000001</v>
@@ -1099,22 +1267,25 @@
       <c r="G19">
         <v>100.751023</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20">
         <v>9.4730729999999994</v>
@@ -1122,22 +1293,25 @@
       <c r="G20">
         <v>100.043656</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21">
         <v>13.755428</v>
@@ -1145,22 +1319,25 @@
       <c r="G21">
         <v>100.62214</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F22">
         <v>13.765029999999999</v>
@@ -1168,22 +1345,25 @@
       <c r="G22">
         <v>100.538877</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F23">
         <v>13.718605999999999</v>
@@ -1191,22 +1371,25 @@
       <c r="G23">
         <v>100.58526500000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="D24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="F24">
         <v>13.718302</v>
@@ -1214,22 +1397,25 @@
       <c r="G24">
         <v>100.589927</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
         <v>79</v>
-      </c>
-      <c r="C25" t="s">
-        <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F25">
         <v>12.564114</v>
@@ -1237,22 +1423,25 @@
       <c r="G25">
         <v>101.45741</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26">
         <v>12.574258</v>
@@ -1260,22 +1449,25 @@
       <c r="G26">
         <v>101.463393</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="F27">
         <v>13.724192</v>
@@ -1283,22 +1475,25 @@
       <c r="G27">
         <v>100.578579</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" t="s">
         <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>87</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28">
         <v>13.719741000000001</v>
@@ -1306,22 +1501,25 @@
       <c r="G28">
         <v>100.576081</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F29">
         <v>13.746867</v>
@@ -1329,28 +1527,112 @@
       <c r="G29">
         <v>100.535037</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
         <v>93</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F30">
         <v>13.740907</v>
       </c>
       <c r="G30">
         <v>100.554479</v>
+      </c>
+      <c r="H30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31">
+        <v>13.825656</v>
+      </c>
+      <c r="G31">
+        <v>100.678804</v>
+      </c>
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32">
+        <v>13.744959</v>
+      </c>
+      <c r="G32">
+        <v>100.54065900000001</v>
+      </c>
+      <c r="H32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33">
+        <v>39.054983999999997</v>
+      </c>
+      <c r="G33">
+        <v>-76.63964</v>
+      </c>
+      <c r="H33" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>